<commit_message>
Rename et fichiers 3D pour assemblage
</commit_message>
<xml_diff>
--- a/009 - References/004-BOM_TOTAL_1V0.xlsx
+++ b/009 - References/004-BOM_TOTAL_1V0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://claurendeau-my.sharepoint.com/personal/yanick_heynemand_claurendeau_qc_ca/Documents/244-57X-AL StrucDocum_A25/Groupe01/PF-109-EP/HapTGP-2025/009 - References/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F1B1DB4-4A5D-4F15-9EC2-326E83BE6F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{7F1B1DB4-4A5D-4F15-9EC2-326E83BE6F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A56BE37-927F-45B4-8E8B-334A0BABB01D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E89EF3B-981F-40AE-B337-2909B44E1F1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="213">
   <si>
     <t>Auteur :</t>
   </si>
@@ -660,6 +660,21 @@
   </si>
   <si>
     <t>https://aliexpi.com/Dnqi</t>
+  </si>
+  <si>
+    <t>En rabais</t>
+  </si>
+  <si>
+    <t>prix unitaire (vient en lot de 100)</t>
+  </si>
+  <si>
+    <t>prix unitaire (vient en lot de 50)</t>
+  </si>
+  <si>
+    <t>prix unitaire (vient en lot de 10)</t>
+  </si>
+  <si>
+    <t>prix unitaire (vient en lot de 96)</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7CBE2E-5CAD-4345-862A-75BBF56E5EAE}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,16 +1220,17 @@
     <col min="1" max="1" width="9.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="2"/>
     <col min="3" max="3" width="49.140625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="20.28515625" style="2"/>
+    <col min="4" max="4" width="20.28515625" style="2"/>
+    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="9" customWidth="1"/>
     <col min="10" max="10" width="35.140625" style="9" customWidth="1"/>
     <col min="11" max="16384" width="20.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
@@ -1228,7 +1244,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1260,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1256,7 +1272,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1288,7 +1304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1321,7 +1337,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1354,7 +1370,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1387,7 +1403,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1420,7 +1436,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1453,7 +1469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1486,7 +1502,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1519,7 +1535,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1552,7 +1568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1585,7 +1601,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1610,15 +1626,18 @@
       <c r="H15" s="13">
         <v>8.99</v>
       </c>
-      <c r="I15" s="14">
-        <f>H15</f>
-        <v>8.99</v>
+      <c r="I15" s="26">
+        <f>H15/96*A15</f>
+        <v>0.37458333333333332</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1641,17 +1660,20 @@
         <v>126</v>
       </c>
       <c r="H16" s="13">
-        <v>30.28</v>
+        <v>9.39</v>
       </c>
       <c r="I16" s="14">
         <f t="shared" si="1"/>
-        <v>30.28</v>
+        <v>9.39</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1684,7 +1706,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1717,7 +1739,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1743,14 +1765,17 @@
         <v>10.99</v>
       </c>
       <c r="I19" s="24">
-        <f t="shared" ref="I19:I25" si="2">H19</f>
-        <v>10.99</v>
+        <f>H19/100*A19</f>
+        <v>0.2198</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1776,14 +1801,17 @@
         <v>2.13</v>
       </c>
       <c r="I20" s="26">
-        <f t="shared" si="2"/>
-        <v>2.13</v>
+        <f>H20/50*A20</f>
+        <v>8.5199999999999998E-2</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1808,15 +1836,18 @@
       <c r="H21" s="13">
         <v>3.07</v>
       </c>
-      <c r="I21" s="24">
-        <f t="shared" si="2"/>
-        <v>3.07</v>
+      <c r="I21" s="26">
+        <f t="shared" ref="I21:I25" si="2">H21/50*A21</f>
+        <v>0.24559999999999998</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1841,15 +1872,18 @@
       <c r="H22" s="13">
         <v>3.48</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I22" s="26">
         <f t="shared" si="2"/>
-        <v>3.48</v>
+        <v>0.13919999999999999</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K22" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1874,15 +1908,18 @@
       <c r="H23" s="13">
         <v>2.13</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="26">
         <f t="shared" si="2"/>
-        <v>2.13</v>
+        <v>0.1704</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1907,15 +1944,18 @@
       <c r="H24" s="13">
         <v>11.49</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="26">
         <f t="shared" si="2"/>
-        <v>11.49</v>
+        <v>0.91920000000000002</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1940,15 +1980,18 @@
       <c r="H25" s="13">
         <v>14.07</v>
       </c>
-      <c r="I25" s="24">
-        <f t="shared" si="2"/>
-        <v>14.07</v>
+      <c r="I25" s="26">
+        <f>H25/10*A25</f>
+        <v>2.8140000000000001</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1981,7 +2024,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2014,7 +2057,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2047,7 +2090,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2080,7 +2123,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2113,7 +2156,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2146,7 +2189,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2522,7 +2565,7 @@
       </c>
       <c r="I43" s="14">
         <f>SUM(I6:I42)</f>
-        <v>157.63999999999999</v>
+        <v>85.367983333333342</v>
       </c>
       <c r="J43" s="18"/>
     </row>
@@ -2539,7 +2582,7 @@
       </c>
       <c r="I44" s="14">
         <f>I43*0.05</f>
-        <v>7.8819999999999997</v>
+        <v>4.2683991666666676</v>
       </c>
       <c r="J44" s="18"/>
     </row>
@@ -2556,7 +2599,7 @@
       </c>
       <c r="I45" s="14">
         <f>I43*0.09975</f>
-        <v>15.724589999999999</v>
+        <v>8.5154563375000016</v>
       </c>
       <c r="J45" s="18"/>
     </row>
@@ -2566,7 +2609,7 @@
       </c>
       <c r="I46" s="19">
         <f>SUM(I43:I45)</f>
-        <v>181.24659</v>
+        <v>98.151838837500009</v>
       </c>
       <c r="J46" s="20"/>
     </row>

</xml_diff>